<commit_message>
refactor: add another version of this function
</commit_message>
<xml_diff>
--- a/Bariants/statgrad-ov-04-29/sg_2020-2021_inf5_18.xlsx
+++ b/Bariants/statgrad-ov-04-29/sg_2020-2021_inf5_18.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htmlprogrammist/Python/ege/EGE/online-olimpiada-ov-04-29/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htmlprogrammist/Python/ege/Bariants/statgrad-ov-04-29/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4577B5A-5F2E-0A40-8937-DD1F48ACAC0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C27925B-D450-6841-981C-F2BF0963588F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{6CF9F464-3206-461F-98B0-C1795E2DDBCA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" xr2:uid="{6CF9F464-3206-461F-98B0-C1795E2DDBCA}"/>
   </bookViews>
   <sheets>
     <sheet name="18" sheetId="5" r:id="rId1"/>
@@ -25,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Ура! Совпало</t>
+  </si>
+  <si>
+    <t>ЕСЛИ(B1&gt;A1;B1+A17;A17)</t>
   </si>
 </sst>
 </file>
@@ -408,7 +411,7 @@
   <dimension ref="A1:W31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1169,6 +1172,11 @@
         <v>16</v>
       </c>
     </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <f>A1</f>

</xml_diff>